<commit_message>
updates metadata with proper date format
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_redd_surveyed_sites_metadata.xlsx
+++ b/data-raw/metadata/feather_redd_surveyed_sites_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\feather-redd\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652C248E-B435-413A-ADAD-EC93531E8393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AFE583-1430-4CA8-BDA8-9E482E32C679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3790" yWindow="1080" windowWidth="15450" windowHeight="12560" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1820" windowWidth="19200" windowHeight="11180" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>surveyed_sites_table</t>
+  </si>
+  <si>
+    <t>whole</t>
   </si>
 </sst>
 </file>
@@ -578,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMF6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -664,6 +667,9 @@
       <c r="G2" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="H2" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J2" s="4"/>
       <c r="K2" s="2"/>
       <c r="L2" s="7">
@@ -727,7 +733,7 @@
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="L5" s="6">
@@ -753,7 +759,7 @@
       <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="L6" s="6">

</xml_diff>